<commit_message>
fix(cdk): batch create template
</commit_message>
<xml_diff>
--- a/source/constructs/config/batch_create/datasource/template/batch_create_jdbc_datasource-cn.xlsx
+++ b/source/constructs/config/batch_create/datasource/template/batch_create_jdbc_datasource-cn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fansu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuihubin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B95DCB-A799-4E4F-AB60-FA930DC7A3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A175F6-6B55-7C43-8E80-08F02B353B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="13300" xr2:uid="{A3F6337F-BB59-9941-91D9-6943CD218DAB}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>SecretARN</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>ProviderID</t>
+  </si>
+  <si>
+    <t>SecretID</t>
   </si>
   <si>
     <t>该模版文件用于批量创建SDP的数据源，请不要修改表头(彩色部分)的信息和顺序。具体规范如下如下：
@@ -76,7 +76,7 @@
 - Description: 选填。
 - JDBC_URL: 必填。数据库实例 格式：jdbc:protocol://host:port。或者，数据库实例中的数据库(database) 格式：jdbc:protocol://host:port/database
 - JDBC_Databases: 选填。如果JDBC_URL填的是mysql协议，此项可保留为空。如果，JDBC_URL填写的是其他数据库实例，请填写相同实例下的数据库中待检测的database，多个database用半角逗号隔开。
-- SecretARN: 选填，secret的ARN。您可以指定SDP所在的AWS账号下的secret manager服务中的secret Id (请提前将用户名/密码存储在此secret中)。
+- SecretID: 选填，secret的ARN。您可以指定SDP所在的AWS账号下的secret manager服务中的secret Id (请提前将用户名/密码存储在此secret中)。
 - Username: 必填。（如果secretID填了，那么此参数将被忽略）
 - Password: 必填。（如果secretID填了，那么此参数将被忽略）
 - AccountID: 请提前在SDP平台添加好账户（account ID），如果账号不存在将报错。
@@ -542,22 +542,22 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11">

</xml_diff>

<commit_message>
update batch create template
</commit_message>
<xml_diff>
--- a/source/constructs/config/batch_create/datasource/template/batch_create_jdbc_datasource-cn.xlsx
+++ b/source/constructs/config/batch_create/datasource/template/batch_create_jdbc_datasource-cn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuihubin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A175F6-6B55-7C43-8E80-08F02B353B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959F849C-FF79-874F-BDBD-42560954007B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="13300" xr2:uid="{A3F6337F-BB59-9941-91D9-6943CD218DAB}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 - Description: 选填。
 - JDBC_URL: 必填。数据库实例 格式：jdbc:protocol://host:port。或者，数据库实例中的数据库(database) 格式：jdbc:protocol://host:port/database
 - JDBC_Databases: 选填。如果JDBC_URL填的是mysql协议，此项可保留为空。如果，JDBC_URL填写的是其他数据库实例，请填写相同实例下的数据库中待检测的database，多个database用半角逗号隔开。
-- SecretID: 选填，secret的ARN。您可以指定SDP所在的AWS账号下的secret manager服务中的secret Id (请提前将用户名/密码存储在此secret中)。
+- SecretID: 选填，secret的ID。您可以指定SDP所在的AWS账号下的secret manager服务中的secret Id (请提前将用户名/密码存储在此secret中)。
 - Username: 必填。（如果secretID填了，那么此参数将被忽略）
 - Password: 必填。（如果secretID填了，那么此参数将被忽略）
 - AccountID: 请提前在SDP平台添加好账户（account ID），如果账号不存在将报错。
@@ -495,7 +495,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>